<commit_message>
Helper to transform competition data for direct use in Pega app
</commit_message>
<xml_diff>
--- a/Product fields for Pega application.xlsx
+++ b/Product fields for Pega application.xlsx
@@ -1,15 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28908"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/perdo/Documents/competitions/kaggle_santander/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="23955" windowHeight="9270"/>
+    <workbookView xWindow="1440" yWindow="3820" windowWidth="31220" windowHeight="14560"/>
   </bookViews>
   <sheets>
     <sheet name="RecordsToCSV_20161212T124822.79" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -791,12 +804,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -826,12 +839,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1035,23 +1048,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="M2" sqref="M2:M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
-    <col min="9" max="10" width="22.5703125" customWidth="1"/>
-    <col min="11" max="11" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="9" max="10" width="22.5" customWidth="1"/>
+    <col min="11" max="11" width="28.5" customWidth="1"/>
     <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1083,15 +1096,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -1101,30 +1114,34 @@
       </c>
       <c r="I2" t="str">
         <f>CONCATENATE("IND_",C2,"_ULT1")</f>
-        <v>IND_CTMA_FIN_ULT1</v>
+        <v>IND_AHOR_FIN_ULT1</v>
       </c>
       <c r="J2" t="str">
         <f>CONCATENATE(".",I2)</f>
-        <v>.IND_CTMA_FIN_ULT1</v>
+        <v>.IND_AHOR_FIN_ULT1</v>
       </c>
       <c r="K2" t="str">
         <f>CONCATENATE("First_",C2)</f>
-        <v>First_CTMA_FIN</v>
+        <v>First_AHOR_FIN</v>
       </c>
       <c r="L2" t="str">
         <f>CONCATENATE("Last_",C2)</f>
-        <v>Last_CTMA_FIN</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Last_AHOR_FIN</v>
+      </c>
+      <c r="M2" t="str">
+        <f>LOWER(I2)</f>
+        <v>ind_ahor_fin_ult1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>25</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -1133,31 +1150,35 @@
         <v>9</v>
       </c>
       <c r="I3" t="str">
-        <f t="shared" ref="I3:I25" si="0">CONCATENATE("IND_",C3,"_ULT1")</f>
-        <v>IND_CTOP_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C3,"_ULT1")</f>
+        <v>IND_AVAL_FIN_ULT1</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J25" si="1">CONCATENATE(".",I3)</f>
-        <v>.IND_CTOP_FIN_ULT1</v>
+        <f>CONCATENATE(".",I3)</f>
+        <v>.IND_AVAL_FIN_ULT1</v>
       </c>
       <c r="K3" t="str">
         <f>CONCATENATE("First_",C3)</f>
-        <v>First_CTOP_FIN</v>
+        <v>First_AVAL_FIN</v>
       </c>
       <c r="L3" t="str">
         <f>CONCATENATE("Last_",C3)</f>
-        <v>Last_CTOP_FIN</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Last_AVAL_FIN</v>
+      </c>
+      <c r="M3" t="str">
+        <f>LOWER(I3)</f>
+        <v>ind_aval_fin_ult1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -1166,31 +1187,35 @@
         <v>9</v>
       </c>
       <c r="I4" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_CTPP_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C4,"_ULT1")</f>
+        <v>IND_CCO_FIN_ULT1</v>
       </c>
       <c r="J4" t="str">
         <f>CONCATENATE(".",I4)</f>
-        <v>.IND_CTPP_FIN_ULT1</v>
+        <v>.IND_CCO_FIN_ULT1</v>
       </c>
       <c r="K4" t="str">
         <f>CONCATENATE("First_",C4)</f>
-        <v>First_CTPP_FIN</v>
+        <v>First_CCO_FIN</v>
       </c>
       <c r="L4" t="str">
         <f>CONCATENATE("Last_",C4)</f>
-        <v>Last_CTPP_FIN</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Last_CCO_FIN</v>
+      </c>
+      <c r="M4" t="str">
+        <f>LOWER(I4)</f>
+        <v>ind_cco_fin_ult1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -1199,31 +1224,35 @@
         <v>9</v>
       </c>
       <c r="I5" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_DECO_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C5,"_ULT1")</f>
+        <v>IND_CDER_FIN_ULT1</v>
       </c>
       <c r="J5" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_DECO_FIN_ULT1</v>
+        <f>CONCATENATE(".",I5)</f>
+        <v>.IND_CDER_FIN_ULT1</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K17" si="2">CONCATENATE("First_",C5)</f>
-        <v>First_DECO_FIN</v>
+        <f>CONCATENATE("First_",C5)</f>
+        <v>First_CDER_FIN</v>
       </c>
       <c r="L5" t="str">
         <f>CONCATENATE("Last_",C5)</f>
-        <v>Last_DECO_FIN</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Last_CDER_FIN</v>
+      </c>
+      <c r="M5" t="str">
+        <f>LOWER(I5)</f>
+        <v>ind_cder_fin_ult1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>31</v>
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="E6" t="s">
         <v>8</v>
@@ -1232,31 +1261,35 @@
         <v>9</v>
       </c>
       <c r="I6" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_DEME_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C6,"_ULT1")</f>
+        <v>IND_CNO_FIN_ULT1</v>
       </c>
       <c r="J6" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_DEME_FIN_ULT1</v>
+        <f>CONCATENATE(".",I6)</f>
+        <v>.IND_CNO_FIN_ULT1</v>
       </c>
       <c r="K6" t="str">
         <f>CONCATENATE("First_",C6)</f>
-        <v>First_DEME_FIN</v>
+        <v>First_CNO_FIN</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" ref="L6:L17" si="3">CONCATENATE("Last_",C6)</f>
-        <v>Last_DEME_FIN</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C6)</f>
+        <v>Last_CNO_FIN</v>
+      </c>
+      <c r="M6" t="str">
+        <f>LOWER(I6)</f>
+        <v>ind_cno_fin_ult1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -1265,31 +1298,35 @@
         <v>9</v>
       </c>
       <c r="I7" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_DELA_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C7,"_ULT1")</f>
+        <v>IND_CTJU_FIN_ULT1</v>
       </c>
       <c r="J7" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_DELA_FIN_ULT1</v>
+        <f>CONCATENATE(".",I7)</f>
+        <v>.IND_CTJU_FIN_ULT1</v>
       </c>
       <c r="K7" t="str">
         <f>CONCATENATE("First_",C7)</f>
-        <v>First_DELA_FIN</v>
+        <v>First_CTJU_FIN</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" si="3"/>
-        <v>Last_DELA_FIN</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C7)</f>
+        <v>Last_CTJU_FIN</v>
+      </c>
+      <c r="M7" t="str">
+        <f>LOWER(I7)</f>
+        <v>ind_ctju_fin_ult1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E8" t="s">
         <v>8</v>
@@ -1298,31 +1335,35 @@
         <v>9</v>
       </c>
       <c r="I8" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_ECUE_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C8,"_ULT1")</f>
+        <v>IND_CTMA_FIN_ULT1</v>
       </c>
       <c r="J8" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_ECUE_FIN_ULT1</v>
+        <f>CONCATENATE(".",I8)</f>
+        <v>.IND_CTMA_FIN_ULT1</v>
       </c>
       <c r="K8" t="str">
-        <f t="shared" si="2"/>
-        <v>First_ECUE_FIN</v>
+        <f>CONCATENATE("First_",C8)</f>
+        <v>First_CTMA_FIN</v>
       </c>
       <c r="L8" t="str">
         <f>CONCATENATE("Last_",C8)</f>
-        <v>Last_ECUE_FIN</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Last_CTMA_FIN</v>
+      </c>
+      <c r="M8" t="str">
+        <f>LOWER(I8)</f>
+        <v>ind_ctma_fin_ult1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="E9" t="s">
         <v>8</v>
@@ -1331,31 +1372,35 @@
         <v>9</v>
       </c>
       <c r="I9" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_FOND_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C9,"_ULT1")</f>
+        <v>IND_CTOP_FIN_ULT1</v>
       </c>
       <c r="J9" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_FOND_FIN_ULT1</v>
+        <f>CONCATENATE(".",I9)</f>
+        <v>.IND_CTOP_FIN_ULT1</v>
       </c>
       <c r="K9" t="str">
-        <f t="shared" si="2"/>
-        <v>First_FOND_FIN</v>
+        <f>CONCATENATE("First_",C9)</f>
+        <v>First_CTOP_FIN</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="3"/>
-        <v>Last_FOND_FIN</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C9)</f>
+        <v>Last_CTOP_FIN</v>
+      </c>
+      <c r="M9" t="str">
+        <f>LOWER(I9)</f>
+        <v>ind_ctop_fin_ult1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
         <v>8</v>
@@ -1364,31 +1409,35 @@
         <v>9</v>
       </c>
       <c r="I10" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_HIP_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C10,"_ULT1")</f>
+        <v>IND_CTPP_FIN_ULT1</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_HIP_FIN_ULT1</v>
+        <f>CONCATENATE(".",I10)</f>
+        <v>.IND_CTPP_FIN_ULT1</v>
       </c>
       <c r="K10" t="str">
-        <f t="shared" si="2"/>
-        <v>First_HIP_FIN</v>
+        <f>CONCATENATE("First_",C10)</f>
+        <v>First_CTPP_FIN</v>
       </c>
       <c r="L10" t="str">
         <f>CONCATENATE("Last_",C10)</f>
-        <v>Last_HIP_FIN</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Last_CTPP_FIN</v>
+      </c>
+      <c r="M10" t="str">
+        <f>LOWER(I10)</f>
+        <v>ind_ctpp_fin_ult1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
         <v>8</v>
@@ -1397,31 +1446,35 @@
         <v>9</v>
       </c>
       <c r="I11" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_PLAN_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C11,"_ULT1")</f>
+        <v>IND_DECO_FIN_ULT1</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_PLAN_FIN_ULT1</v>
+        <f>CONCATENATE(".",I11)</f>
+        <v>.IND_DECO_FIN_ULT1</v>
       </c>
       <c r="K11" t="str">
         <f>CONCATENATE("First_",C11)</f>
-        <v>First_PLAN_FIN</v>
+        <v>First_DECO_FIN</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="3"/>
-        <v>Last_PLAN_FIN</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C11)</f>
+        <v>Last_DECO_FIN</v>
+      </c>
+      <c r="M11" t="str">
+        <f>LOWER(I11)</f>
+        <v>ind_deco_fin_ult1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
@@ -1430,31 +1483,35 @@
         <v>9</v>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_PRES_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C12,"_ULT1")</f>
+        <v>IND_DELA_FIN_ULT1</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_PRES_FIN_ULT1</v>
+        <f>CONCATENATE(".",I12)</f>
+        <v>.IND_DELA_FIN_ULT1</v>
       </c>
       <c r="K12" t="str">
         <f>CONCATENATE("First_",C12)</f>
-        <v>First_PRES_FIN</v>
+        <v>First_DELA_FIN</v>
       </c>
       <c r="L12" t="str">
         <f>CONCATENATE("Last_",C12)</f>
-        <v>Last_PRES_FIN</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Last_DELA_FIN</v>
+      </c>
+      <c r="M12" t="str">
+        <f>LOWER(I12)</f>
+        <v>ind_dela_fin_ult1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1463,31 +1520,35 @@
         <v>9</v>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_RECA_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C13,"_ULT1")</f>
+        <v>IND_DEME_FIN_ULT1</v>
       </c>
       <c r="J13" t="str">
         <f>CONCATENATE(".",I13)</f>
-        <v>.IND_RECA_FIN_ULT1</v>
+        <v>.IND_DEME_FIN_ULT1</v>
       </c>
       <c r="K13" t="str">
-        <f t="shared" si="2"/>
-        <v>First_RECA_FIN</v>
+        <f>CONCATENATE("First_",C13)</f>
+        <v>First_DEME_FIN</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="3"/>
-        <v>Last_RECA_FIN</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C13)</f>
+        <v>Last_DEME_FIN</v>
+      </c>
+      <c r="M13" t="str">
+        <f>LOWER(I13)</f>
+        <v>ind_deme_fin_ult1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
         <v>8</v>
@@ -1496,31 +1557,35 @@
         <v>9</v>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_TJCR_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C14,"_ULT1")</f>
+        <v>IND_ECUE_FIN_ULT1</v>
       </c>
       <c r="J14" t="str">
         <f>CONCATENATE(".",I14)</f>
-        <v>.IND_TJCR_FIN_ULT1</v>
+        <v>.IND_ECUE_FIN_ULT1</v>
       </c>
       <c r="K14" t="str">
-        <f t="shared" si="2"/>
-        <v>First_TJCR_FIN</v>
+        <f>CONCATENATE("First_",C14)</f>
+        <v>First_ECUE_FIN</v>
       </c>
       <c r="L14" t="str">
         <f>CONCATENATE("Last_",C14)</f>
-        <v>Last_TJCR_FIN</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Last_ECUE_FIN</v>
+      </c>
+      <c r="M14" t="str">
+        <f>LOWER(I14)</f>
+        <v>ind_ecue_fin_ult1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -1529,31 +1594,35 @@
         <v>9</v>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_VALO_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C15,"_ULT1")</f>
+        <v>IND_FOND_FIN_ULT1</v>
       </c>
       <c r="J15" t="str">
         <f>CONCATENATE(".",I15)</f>
-        <v>.IND_VALO_FIN_ULT1</v>
+        <v>.IND_FOND_FIN_ULT1</v>
       </c>
       <c r="K15" t="str">
         <f>CONCATENATE("First_",C15)</f>
-        <v>First_VALO_FIN</v>
+        <v>First_FOND_FIN</v>
       </c>
       <c r="L15" t="str">
         <f>CONCATENATE("Last_",C15)</f>
-        <v>Last_VALO_FIN</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>Last_FOND_FIN</v>
+      </c>
+      <c r="M15" t="str">
+        <f>LOWER(I15)</f>
+        <v>ind_fond_fin_ult1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
@@ -1562,97 +1631,109 @@
         <v>9</v>
       </c>
       <c r="I16" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_VIV_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C16,"_ULT1")</f>
+        <v>IND_HIP_FIN_ULT1</v>
       </c>
       <c r="J16" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_VIV_FIN_ULT1</v>
+        <f>CONCATENATE(".",I16)</f>
+        <v>.IND_HIP_FIN_ULT1</v>
       </c>
       <c r="K16" t="str">
-        <f t="shared" si="2"/>
-        <v>First_VIV_FIN</v>
+        <f>CONCATENATE("First_",C16)</f>
+        <v>First_HIP_FIN</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="3"/>
-        <v>Last_VIV_FIN</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C16)</f>
+        <v>Last_HIP_FIN</v>
+      </c>
+      <c r="M16" t="str">
+        <f>LOWER(I16)</f>
+        <v>ind_hip_fin_ult1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
       <c r="B17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" t="str">
+        <f>CONCATENATE("IND_",C17,"_ULT1")</f>
+        <v>IND_NOM_PENS_ULT1</v>
+      </c>
+      <c r="J17" t="str">
+        <f>CONCATENATE(".",I17)</f>
+        <v>.IND_NOM_PENS_ULT1</v>
+      </c>
+      <c r="K17" t="str">
+        <f>CONCATENATE("First_",C17)</f>
+        <v>First_NOM_PENS</v>
+      </c>
+      <c r="L17" t="str">
+        <f>CONCATENATE("Last_",C17)</f>
+        <v>Last_NOM_PENS</v>
+      </c>
+      <c r="M17" t="str">
+        <f>LOWER(I17)</f>
+        <v>ind_nom_pens_ult1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" t="s">
-        <v>9</v>
-      </c>
-      <c r="I17" t="str">
-        <f t="shared" si="0"/>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" t="str">
+        <f>CONCATENATE("IND_",C18,"_ULT1")</f>
         <v>IND_NOMINA_ULT1</v>
       </c>
-      <c r="J17" t="str">
-        <f t="shared" si="1"/>
+      <c r="J18" t="str">
+        <f>CONCATENATE(".",I18)</f>
         <v>.IND_NOMINA_ULT1</v>
       </c>
-      <c r="K17" t="str">
-        <f t="shared" si="2"/>
+      <c r="K18" t="str">
+        <f>CONCATENATE("First_",C18)</f>
         <v>First_NOMINA</v>
       </c>
-      <c r="L17" t="str">
-        <f t="shared" si="3"/>
+      <c r="L18" t="str">
+        <f>CONCATENATE("Last_",C18)</f>
         <v>Last_NOMINA</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" t="s">
-        <v>9</v>
-      </c>
-      <c r="I18" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_AHOR_FIN_ULT1</v>
-      </c>
-      <c r="J18" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_AHOR_FIN_ULT1</v>
-      </c>
-      <c r="K18" t="str">
-        <f t="shared" ref="K18:K25" si="4">CONCATENATE("First_",C18)</f>
-        <v>First_AHOR_FIN</v>
-      </c>
-      <c r="L18" t="str">
-        <f t="shared" ref="L18:L25" si="5">CONCATENATE("Last_",C18)</f>
-        <v>Last_AHOR_FIN</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="str">
+        <f>LOWER(I18)</f>
+        <v>ind_nomina_ult1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>13</v>
+        <v>40</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="E19" t="s">
         <v>8</v>
@@ -1661,31 +1742,35 @@
         <v>9</v>
       </c>
       <c r="I19" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_AVAL_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C19,"_ULT1")</f>
+        <v>IND_PLAN_FIN_ULT1</v>
       </c>
       <c r="J19" t="str">
         <f>CONCATENATE(".",I19)</f>
-        <v>.IND_AVAL_FIN_ULT1</v>
+        <v>.IND_PLAN_FIN_ULT1</v>
       </c>
       <c r="K19" t="str">
-        <f t="shared" si="4"/>
-        <v>First_AVAL_FIN</v>
+        <f>CONCATENATE("First_",C19)</f>
+        <v>First_PLAN_FIN</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" si="5"/>
-        <v>Last_AVAL_FIN</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C19)</f>
+        <v>Last_PLAN_FIN</v>
+      </c>
+      <c r="M19" t="str">
+        <f>LOWER(I19)</f>
+        <v>ind_plan_fin_ult1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="E20" t="s">
         <v>8</v>
@@ -1694,31 +1779,35 @@
         <v>9</v>
       </c>
       <c r="I20" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_CCO_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C20,"_ULT1")</f>
+        <v>IND_PRES_FIN_ULT1</v>
       </c>
       <c r="J20" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_CCO_FIN_ULT1</v>
+        <f>CONCATENATE(".",I20)</f>
+        <v>.IND_PRES_FIN_ULT1</v>
       </c>
       <c r="K20" t="str">
-        <f t="shared" si="4"/>
-        <v>First_CCO_FIN</v>
+        <f>CONCATENATE("First_",C20)</f>
+        <v>First_PRES_FIN</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="5"/>
-        <v>Last_CCO_FIN</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C20)</f>
+        <v>Last_PRES_FIN</v>
+      </c>
+      <c r="M20" t="str">
+        <f>LOWER(I20)</f>
+        <v>ind_pres_fin_ult1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>17</v>
+        <v>44</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E21" t="s">
         <v>8</v>
@@ -1727,31 +1816,35 @@
         <v>9</v>
       </c>
       <c r="I21" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_CDER_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C21,"_ULT1")</f>
+        <v>IND_RECA_FIN_ULT1</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_CDER_FIN_ULT1</v>
+        <f>CONCATENATE(".",I21)</f>
+        <v>.IND_RECA_FIN_ULT1</v>
       </c>
       <c r="K21" t="str">
-        <f t="shared" si="4"/>
-        <v>First_CDER_FIN</v>
+        <f>CONCATENATE("First_",C21)</f>
+        <v>First_RECA_FIN</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" si="5"/>
-        <v>Last_CDER_FIN</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C21)</f>
+        <v>Last_RECA_FIN</v>
+      </c>
+      <c r="M21" t="str">
+        <f>LOWER(I21)</f>
+        <v>ind_reca_fin_ult1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1760,31 +1853,35 @@
         <v>9</v>
       </c>
       <c r="I22" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_CNO_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C22,"_ULT1")</f>
+        <v>IND_RECIBO_ULT1</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_CNO_FIN_ULT1</v>
+        <f>CONCATENATE(".",I22)</f>
+        <v>.IND_RECIBO_ULT1</v>
       </c>
       <c r="K22" t="str">
-        <f t="shared" si="4"/>
-        <v>First_CNO_FIN</v>
+        <f>CONCATENATE("First_",C22)</f>
+        <v>First_RECIBO</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="5"/>
-        <v>Last_CNO_FIN</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C22)</f>
+        <v>Last_RECIBO</v>
+      </c>
+      <c r="M22" t="str">
+        <f>LOWER(I22)</f>
+        <v>ind_recibo_ult1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="E23" t="s">
         <v>8</v>
@@ -1793,31 +1890,35 @@
         <v>9</v>
       </c>
       <c r="I23" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_CTJU_FIN_ULT1</v>
+        <f>CONCATENATE("IND_",C23,"_ULT1")</f>
+        <v>IND_TJCR_FIN_ULT1</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_CTJU_FIN_ULT1</v>
+        <f>CONCATENATE(".",I23)</f>
+        <v>.IND_TJCR_FIN_ULT1</v>
       </c>
       <c r="K23" t="str">
-        <f t="shared" si="4"/>
-        <v>First_CTJU_FIN</v>
+        <f>CONCATENATE("First_",C23)</f>
+        <v>First_TJCR_FIN</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="5"/>
-        <v>Last_CTJU_FIN</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C23)</f>
+        <v>Last_TJCR_FIN</v>
+      </c>
+      <c r="M23" t="str">
+        <f>LOWER(I23)</f>
+        <v>ind_tjcr_fin_ult1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1826,31 +1927,35 @@
         <v>9</v>
       </c>
       <c r="I24" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_NOM_PENS_ULT1</v>
+        <f>CONCATENATE("IND_",C24,"_ULT1")</f>
+        <v>IND_VALO_FIN_ULT1</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_NOM_PENS_ULT1</v>
+        <f>CONCATENATE(".",I24)</f>
+        <v>.IND_VALO_FIN_ULT1</v>
       </c>
       <c r="K24" t="str">
-        <f t="shared" si="4"/>
-        <v>First_NOM_PENS</v>
+        <f>CONCATENATE("First_",C24)</f>
+        <v>First_VALO_FIN</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="5"/>
-        <v>Last_NOM_PENS</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C24)</f>
+        <v>Last_VALO_FIN</v>
+      </c>
+      <c r="M24" t="str">
+        <f>LOWER(I24)</f>
+        <v>ind_valo_fin_ult1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="E25" t="s">
         <v>8</v>
@@ -1859,28 +1964,35 @@
         <v>9</v>
       </c>
       <c r="I25" t="str">
-        <f t="shared" si="0"/>
-        <v>IND_RECIBO_ULT1</v>
+        <f>CONCATENATE("IND_",C25,"_ULT1")</f>
+        <v>IND_VIV_FIN_ULT1</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" si="1"/>
-        <v>.IND_RECIBO_ULT1</v>
+        <f>CONCATENATE(".",I25)</f>
+        <v>.IND_VIV_FIN_ULT1</v>
       </c>
       <c r="K25" t="str">
-        <f t="shared" si="4"/>
-        <v>First_RECIBO</v>
+        <f>CONCATENATE("First_",C25)</f>
+        <v>First_VIV_FIN</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" si="5"/>
-        <v>Last_RECIBO</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <f>CONCATENATE("Last_",C25)</f>
+        <v>Last_VIV_FIN</v>
+      </c>
+      <c r="M25" t="str">
+        <f>LOWER(I25)</f>
+        <v>ind_viv_fin_ult1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K26" s="2" t="s">
         <v>57</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:M26">
+    <sortCondition ref="M2:M26"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>